<commit_message>
ADDED MEMBER_USERCONTROL, MEMBER_NEW_USERCONTROL, FINISHED IMPORT_MEMBERS FROM EXCEL FILE, MEMBER PICS TABLE ADDED TO DATABASE.
</commit_message>
<xml_diff>
--- a/MMG-PIAPS/bin/Debug/Membership.xlsx
+++ b/MMG-PIAPS/bin/Debug/Membership.xlsx
@@ -1311,7 +1311,7 @@
   <dimension ref="A1:K251"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6368,6 +6368,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="W1:W2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="S1:T1"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="A1:A2"/>
@@ -6375,13 +6382,6 @@
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:H1"/>
-    <mergeCell ref="V1:V2"/>
-    <mergeCell ref="W1:W2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="S1:T1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>